<commit_message>
Updated the websocket timeout
</commit_message>
<xml_diff>
--- a/REDIS.xlsx
+++ b/REDIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SACMES_web\web\SACMES_Web-Multiuser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206E75F2-CD00-4D80-B63E-61F0D90AD8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52D47DF-A3FF-4802-9ABA-8727156FEF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,7 +367,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>